<commit_message>
chore(example): refresh nightfall data tables
</commit_message>
<xml_diff>
--- a/example/game_06_abyssal_nightfall/enemies.xlsx
+++ b/example/game_06_abyssal_nightfall/enemies.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:S9"/>
+  <dimension ref="A4:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -460,6 +460,9 @@
       <c r="S4" t="str">
         <v>string</v>
       </c>
+      <c r="T4" t="str">
+        <v>uint</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -519,6 +522,9 @@
       <c r="S5" t="str">
         <v>combatNotes</v>
       </c>
+      <c r="T5" t="str">
+        <v>xp</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -578,6 +584,9 @@
       <c r="S6" t="str">
         <v>Lobs corrupted bile; projectile arc 35 degrees.</v>
       </c>
+      <c r="T6" t="str">
+        <v>18</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -637,6 +646,9 @@
       <c r="S7" t="str">
         <v>Fires 3-note burst; third note inflicts dread stack.</v>
       </c>
+      <c r="T7" t="str">
+        <v>26</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -696,6 +708,9 @@
       <c r="S8" t="str">
         <v>Line cone shockwave; adds sanity bleed over 3s.</v>
       </c>
+      <c r="T8" t="str">
+        <v>32</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -755,10 +770,137 @@
       <c r="S9" t="str">
         <v>Sweeping beam telegraph 0.6s; pierces obstacles.</v>
       </c>
+      <c r="T9" t="str">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>40</v>
+      </c>
+      <c r="B10" t="str">
+        <v>06</v>
+      </c>
+      <c r="C10" t="str">
+        <v>0005</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Harbor Dredger</v>
+      </c>
+      <c r="E10" t="str">
+        <v>CONSTRUCT</v>
+      </c>
+      <c r="F10" t="str">
+        <v>520</v>
+      </c>
+      <c r="G10" t="str">
+        <v>55</v>
+      </c>
+      <c r="H10" t="str">
+        <v>2.2</v>
+      </c>
+      <c r="I10" t="str">
+        <v>MANUAL</v>
+      </c>
+      <c r="J10" t="str">
+        <v>1.10</v>
+      </c>
+      <c r="K10" t="str">
+        <v>0</v>
+      </c>
+      <c r="L10" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="M10" t="str">
+        <v>fx/projectiles/dredger_slam.png</v>
+      </c>
+      <c r="N10" t="str">
+        <v>fx/impact/dredger_slam.png</v>
+      </c>
+      <c r="O10" t="str">
+        <v>FIRE</v>
+      </c>
+      <c r="P10" t="str">
+        <v>KINETIC</v>
+      </c>
+      <c r="Q10" t="str">
+        <v>loot:dredger_core</v>
+      </c>
+      <c r="R10" t="str">
+        <v>14</v>
+      </c>
+      <c r="S10" t="str">
+        <v>Heavy mech charges the beacon and causes shock tremors.</v>
+      </c>
+      <c r="T10" t="str">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>40</v>
+      </c>
+      <c r="B11" t="str">
+        <v>06</v>
+      </c>
+      <c r="C11" t="str">
+        <v>0006</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Myriad Fragment</v>
+      </c>
+      <c r="E11" t="str">
+        <v>ABERRATION</v>
+      </c>
+      <c r="F11" t="str">
+        <v>160</v>
+      </c>
+      <c r="G11" t="str">
+        <v>18</v>
+      </c>
+      <c r="H11" t="str">
+        <v>4.8</v>
+      </c>
+      <c r="I11" t="str">
+        <v>BURST</v>
+      </c>
+      <c r="J11" t="str">
+        <v>1.90</v>
+      </c>
+      <c r="K11" t="str">
+        <v>26</v>
+      </c>
+      <c r="L11" t="str">
+        <v>0.75</v>
+      </c>
+      <c r="M11" t="str">
+        <v>fx/projectiles/fragment_dart.png</v>
+      </c>
+      <c r="N11" t="str">
+        <v>fx/impact/fragment_spark.png</v>
+      </c>
+      <c r="O11" t="str">
+        <v>LIGHT</v>
+      </c>
+      <c r="P11" t="str">
+        <v>VOID</v>
+      </c>
+      <c r="Q11" t="str">
+        <v>loot:fragment_cache</v>
+      </c>
+      <c r="R11" t="str">
+        <v>8</v>
+      </c>
+      <c r="S11" t="str">
+        <v>Skittering shards fire dart volleys in packs.</v>
+      </c>
+      <c r="T11" t="str">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A4:S9"/>
+    <ignoredError numberStoredAsText="1" sqref="A4:T11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: ease opening waves and refresh skill visuals
</commit_message>
<xml_diff>
--- a/example/game_06_abyssal_nightfall/enemies.xlsx
+++ b/example/game_06_abyssal_nightfall/enemies.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:Z11"/>
+  <dimension ref="A4:Z12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -597,7 +597,7 @@
         <v>1.80</v>
       </c>
       <c r="L6" t="str">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="M6" t="str">
         <v>0.90</v>
@@ -627,7 +627,7 @@
         <v>18</v>
       </c>
       <c r="V6" t="str">
-        <v>ui/assets/topdown/top-down-shooter/characters/head/13.png</v>
+        <v>ui/assets/topdown/top-down-shooter/characters/body/3.png</v>
       </c>
       <c r="W6" t="str">
         <v>0.9</v>
@@ -707,10 +707,10 @@
         <v>26</v>
       </c>
       <c r="V7" t="str">
-        <v>ui/assets/topdown/top-down-shooter/characters/head/7.png</v>
+        <v>ui/assets/topdown/top-down-shooter/characters/body/2.png</v>
       </c>
       <c r="W7" t="str">
-        <v>0.92</v>
+        <v>0.94</v>
       </c>
       <c r="X7" t="str">
         <v>ui/assets/topdown/top-down-shooter/effects/4.png</v>
@@ -745,22 +745,22 @@
         <v>36</v>
       </c>
       <c r="H8" t="str">
-        <v>4.0</v>
+        <v>3.6</v>
       </c>
       <c r="I8" t="str">
         <v>16</v>
       </c>
       <c r="J8" t="str">
-        <v>MANUAL</v>
+        <v>BURST</v>
       </c>
       <c r="K8" t="str">
-        <v>2.80</v>
+        <v>2.60</v>
       </c>
       <c r="L8" t="str">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="M8" t="str">
-        <v>0.00</v>
+        <v>0.70</v>
       </c>
       <c r="N8" t="str">
         <v>fx/projectiles/howl_wave.png</v>
@@ -787,10 +787,10 @@
         <v>32</v>
       </c>
       <c r="V8" t="str">
-        <v>ui/assets/topdown/top-down-shooter/characters/head/4.png</v>
+        <v>ui/assets/topdown/top-down-shooter/characters/body/1.png</v>
       </c>
       <c r="W8" t="str">
-        <v>0.95</v>
+        <v>0.92</v>
       </c>
       <c r="X8" t="str">
         <v>ui/assets/topdown/top-down-shooter/effects/3.png</v>
@@ -837,10 +837,10 @@
         <v>1.45</v>
       </c>
       <c r="L9" t="str">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="M9" t="str">
-        <v>0.50</v>
+        <v>0.60</v>
       </c>
       <c r="N9" t="str">
         <v>fx/projectiles/null_beam.png</v>
@@ -867,7 +867,7 @@
         <v>38</v>
       </c>
       <c r="V9" t="str">
-        <v>ui/assets/topdown/top-down-shooter/characters/turret/1.png</v>
+        <v>ui/assets/topdown/top-down-shooter/characters/turret/2.png</v>
       </c>
       <c r="W9" t="str">
         <v>1.05</v>
@@ -979,13 +979,13 @@
         <v>ABERRATION</v>
       </c>
       <c r="F11" t="str">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="G11" t="str">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H11" t="str">
-        <v>4.8</v>
+        <v>3.6</v>
       </c>
       <c r="I11" t="str">
         <v>10</v>
@@ -994,13 +994,13 @@
         <v>BURST</v>
       </c>
       <c r="K11" t="str">
-        <v>1.90</v>
+        <v>2.40</v>
       </c>
       <c r="L11" t="str">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="M11" t="str">
-        <v>0.75</v>
+        <v>0.90</v>
       </c>
       <c r="N11" t="str">
         <v>fx/projectiles/fragment_dart.png</v>
@@ -1018,19 +1018,19 @@
         <v>loot:fragment_cache</v>
       </c>
       <c r="S11" t="str">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="T11" t="str">
-        <v>群猎碎片成群而行，形成交叉弹雨。</v>
+        <v>碎影快速游走射击，首波练习走位。</v>
       </c>
       <c r="U11" t="str">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="V11" t="str">
-        <v>ui/assets/topdown/top-down-shooter/effects/1.png</v>
+        <v>ui/assets/topdown/top-down-shooter/characters/head/9.png</v>
       </c>
       <c r="W11" t="str">
-        <v>1.0</v>
+        <v>0.8</v>
       </c>
       <c r="X11" t="str">
         <v>ui/assets/topdown/top-down-shooter/effects/2.png</v>
@@ -1040,11 +1040,91 @@
       </c>
       <c r="Z11" t="str">
         <v>ui/assets/topdown/top-down-shooter/sounds/shoot-1.wav</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>40</v>
+      </c>
+      <c r="B12" t="str">
+        <v>06</v>
+      </c>
+      <c r="C12" t="str">
+        <v>0007</v>
+      </c>
+      <c r="D12" t="str">
+        <v>虚潮行者</v>
+      </c>
+      <c r="E12" t="str">
+        <v>SHAMBLER</v>
+      </c>
+      <c r="F12" t="str">
+        <v>150</v>
+      </c>
+      <c r="G12" t="str">
+        <v>12</v>
+      </c>
+      <c r="H12" t="str">
+        <v>2.9</v>
+      </c>
+      <c r="I12" t="str">
+        <v>16</v>
+      </c>
+      <c r="J12" t="str">
+        <v>MANUAL</v>
+      </c>
+      <c r="K12" t="str">
+        <v>0</v>
+      </c>
+      <c r="L12" t="str">
+        <v>0</v>
+      </c>
+      <c r="M12" t="str">
+        <v>0</v>
+      </c>
+      <c r="N12" t="str">
+        <v/>
+      </c>
+      <c r="O12" t="str">
+        <v/>
+      </c>
+      <c r="P12" t="str">
+        <v>LIGHT</v>
+      </c>
+      <c r="Q12" t="str">
+        <v>VOID</v>
+      </c>
+      <c r="R12" t="str">
+        <v>loot:ichor_minor</v>
+      </c>
+      <c r="S12" t="str">
+        <v>4</v>
+      </c>
+      <c r="T12" t="str">
+        <v>只会贴身缠斗的虚潮行者，用来熟悉位移。</v>
+      </c>
+      <c r="U12" t="str">
+        <v>14</v>
+      </c>
+      <c r="V12" t="str">
+        <v>ui/assets/topdown/top-down-shooter/characters/head/5.png</v>
+      </c>
+      <c r="W12" t="str">
+        <v>0.88</v>
+      </c>
+      <c r="X12" t="str">
+        <v>ui/assets/topdown/top-down-shooter/effects/explosion.png</v>
+      </c>
+      <c r="Y12" t="str">
+        <v>ui/assets/topdown/top-down-shooter/sounds/death.wav</v>
+      </c>
+      <c r="Z12" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A4:Z11"/>
+    <ignoredError numberStoredAsText="1" sqref="A4:Z12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>